<commit_message>
added some etxra sensors
</commit_message>
<xml_diff>
--- a/nameConversion.xlsx
+++ b/nameConversion.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neilwhite/Library/CloudStorage/Dropbox/BitBucket/priva_dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A47641E7-6D8D-E148-88A1-F9DC2D030999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB30E424-9DDC-4547-92E7-CBA017A8A509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3980" yWindow="-20380" windowWidth="27640" windowHeight="16940" xr2:uid="{11CEF6D7-D590-FE48-B7E9-BAF3D753B8DE}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20120" xr2:uid="{11CEF6D7-D590-FE48-B7E9-BAF3D753B8DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Names" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="152">
   <si>
     <t>800000a1-0001-0001-0000-0000800013b0</t>
   </si>
@@ -456,6 +456,42 @@
   </si>
   <si>
     <t>Pretty</t>
+  </si>
+  <si>
+    <t>8000008c-0001-0001-0000-000080000a74</t>
+  </si>
+  <si>
+    <t>Desired_EC</t>
+  </si>
+  <si>
+    <t>Measured_EC</t>
+  </si>
+  <si>
+    <t> 8000008f-0001-8101-0000-0000800007c5</t>
+  </si>
+  <si>
+    <t>Desired_pH_1</t>
+  </si>
+  <si>
+    <t> 8000008f-0001-8101-0000-0000800007f3</t>
+  </si>
+  <si>
+    <t>Measured_pH_1</t>
+  </si>
+  <si>
+    <t> 8000008f-0001-8201-0000-0000800007c5</t>
+  </si>
+  <si>
+    <t>Desired_pH_2</t>
+  </si>
+  <si>
+    <t> 8000008f-0001-8201-0000-0000800007f3</t>
+  </si>
+  <si>
+    <t>Measured_pH_2</t>
+  </si>
+  <si>
+    <t>8000008c-0001-0001-0000-000080000a7d</t>
   </si>
 </sst>
 </file>
@@ -823,15 +859,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5521EBDD-71F0-7546-9ADE-A6E042F48762}">
-  <dimension ref="A1:B70"/>
+  <dimension ref="A1:B76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40" customWidth="1"/>
+    <col min="1" max="1" width="50.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1395,7 +1431,56 @@
         <v>137</v>
       </c>
     </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>140</v>
+      </c>
+      <c r="B71" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>151</v>
+      </c>
+      <c r="B72" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>143</v>
+      </c>
+      <c r="B73" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>145</v>
+      </c>
+      <c r="B74" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>147</v>
+      </c>
+      <c r="B75" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>149</v>
+      </c>
+      <c r="B76" t="s">
+        <v>150</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
extra dosing channels and list of all available datapoints
</commit_message>
<xml_diff>
--- a/nameConversion.xlsx
+++ b/nameConversion.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neilwhite/Library/CloudStorage/Dropbox/BitBucket/priva_dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA3048E-030A-4242-BDF8-542D73249A3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8CFEE1-AFAB-7046-9B0B-BFF6D7207A85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20080" xr2:uid="{11CEF6D7-D590-FE48-B7E9-BAF3D753B8DE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="158">
   <si>
     <t>800000a1-0001-0001-0000-0000800013b0</t>
   </si>
@@ -492,13 +492,31 @@
   </si>
   <si>
     <t>8000008f-0001-8201-0000-0000800007f3</t>
+  </si>
+  <si>
+    <t>8000008c-0001-0001-0000-000080000a77</t>
+  </si>
+  <si>
+    <t>8000008f-0001-8101-0000-0000800007d3</t>
+  </si>
+  <si>
+    <t>Dosing_pH_1</t>
+  </si>
+  <si>
+    <t>Dosing_EC</t>
+  </si>
+  <si>
+    <t>Dosing_pH_2</t>
+  </si>
+  <si>
+    <t>8000008f-0001-8201-0000-0000800007d3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -519,6 +537,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFCE9178"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -541,10 +565,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -859,11 +884,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5521EBDD-71F0-7546-9ADE-A6E042F48762}">
-  <dimension ref="A1:B76"/>
+  <dimension ref="A1:B80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1479,6 +1502,33 @@
         <v>146</v>
       </c>
     </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>152</v>
+      </c>
+      <c r="B77" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>153</v>
+      </c>
+      <c r="B78" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>157</v>
+      </c>
+      <c r="B79" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
updates for outside temperature
</commit_message>
<xml_diff>
--- a/nameConversion.xlsx
+++ b/nameConversion.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neilwhite/Library/CloudStorage/Dropbox/BitBucket/priva_dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8CFEE1-AFAB-7046-9B0B-BFF6D7207A85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC28F8E-7CD2-0042-9E7B-E83B6F1B41DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20080" xr2:uid="{11CEF6D7-D590-FE48-B7E9-BAF3D753B8DE}"/>
+    <workbookView xWindow="51200" yWindow="500" windowWidth="25600" windowHeight="28300" xr2:uid="{11CEF6D7-D590-FE48-B7E9-BAF3D753B8DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Names" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="170">
   <si>
     <t>800000a1-0001-0001-0000-0000800013b0</t>
   </si>
@@ -510,6 +510,42 @@
   </si>
   <si>
     <t>8000008f-0001-8201-0000-0000800007d3</t>
+  </si>
+  <si>
+    <t>8000009f-0001-0001-0000-0000800012ec</t>
+  </si>
+  <si>
+    <t>80da33e1-cd0d-479e-9628-70bcccdb304e</t>
+  </si>
+  <si>
+    <t>Outside_Air_Temperature</t>
+  </si>
+  <si>
+    <t>Outside_Relative_Humidity</t>
+  </si>
+  <si>
+    <t>800000a0-0001-0001-0000-0000800012d1</t>
+  </si>
+  <si>
+    <t>Outside_Light_Intensity</t>
+  </si>
+  <si>
+    <t>Outside_Light_Accumulation_Today</t>
+  </si>
+  <si>
+    <t>800000a1-0001-0001-0000-0000800013a5</t>
+  </si>
+  <si>
+    <t>Outside_Light_Accumulation_Last24Hrs</t>
+  </si>
+  <si>
+    <t>800000e3-0001-0001-0000-000080002252</t>
+  </si>
+  <si>
+    <t>Outside_Pressure_kPa</t>
+  </si>
+  <si>
+    <t>Outside_Pressure_Change_kPa</t>
   </si>
 </sst>
 </file>
@@ -534,23 +570,29 @@
     </font>
     <font>
       <sz val="12"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FFCE9178"/>
+      <color rgb="FFA31515"/>
       <name val="Menlo"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -562,16 +604,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -884,13 +928,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5521EBDD-71F0-7546-9ADE-A6E042F48762}">
-  <dimension ref="A1:B80"/>
+  <dimension ref="A1:B86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="A80" sqref="A80"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1159,7 +1205,7 @@
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="A34" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -1183,10 +1229,10 @@
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="A37" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="2" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1527,7 +1573,60 @@
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A80" s="3"/>
+      <c r="A80" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B80" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B81" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B82" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B83" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B84" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B85" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B86" t="s">
+        <v>169</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>